<commit_message>
23 Nov 23 Development
</commit_message>
<xml_diff>
--- a/Extraction_PO_Data_IntoCSV/Data/Config.xlsx
+++ b/Extraction_PO_Data_IntoCSV/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa.uat\Documents\UiPath\SH-Cogent\Extraction_PO_Data_IntoCSV\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D76F0180-F5C6-446D-9628-85434DA29A6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5445A33F-C61A-4EC5-A11D-3CFA831698E3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="87">
   <si>
     <t>Name</t>
   </si>
@@ -216,9 +216,6 @@
     <t>StatusTrackerFileName</t>
   </si>
   <si>
-    <t>Data\Output\Status Tracker.xlsx</t>
-  </si>
-  <si>
     <t>StatusTracker_TemplateFile</t>
   </si>
   <si>
@@ -253,6 +250,42 @@
   </si>
   <si>
     <t>Data\Input\Template\Line Item Template.xlsx</t>
+  </si>
+  <si>
+    <t>ExcpMsg_TotalbefGSTEmpty</t>
+  </si>
+  <si>
+    <t>Total before GST Or To be Del Value or To be inv Value is empty</t>
+  </si>
+  <si>
+    <t>Data\Output\CSV_StatusTracker_</t>
+  </si>
+  <si>
+    <t>SAP_LogonPath</t>
+  </si>
+  <si>
+    <t>C:\Program Files (x86)\SAP\FrontEnd\SAPgui\saplogon.exe</t>
+  </si>
+  <si>
+    <t>ConnectionName</t>
+  </si>
+  <si>
+    <t>DEV</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>SAP_Credential</t>
+  </si>
+  <si>
+    <t>SAP_Cred</t>
+  </si>
+  <si>
+    <t>ExcpMsg_ReportnoReady</t>
+  </si>
+  <si>
+    <t>Report not ready to download</t>
   </si>
 </sst>
 </file>
@@ -631,7 +664,7 @@
   <dimension ref="A1:Z998"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -709,10 +742,38 @@
       </c>
     </row>
     <row r="6" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="7" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="8" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="9" spans="1:26" ht="14.25" customHeight="1"/>
-    <row r="10" spans="1:26" ht="14.25" customHeight="1"/>
+    <row r="7" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A7" t="s">
+        <v>78</v>
+      </c>
+      <c r="B7" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A8" t="s">
+        <v>80</v>
+      </c>
+      <c r="B8" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9">
+        <v>800</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10" t="s">
+        <v>84</v>
+      </c>
+    </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="12" spans="1:26" ht="14.25" customHeight="1"/>
     <row r="13" spans="1:26" ht="14.25" customHeight="1"/>
@@ -1710,10 +1771,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:Z989"/>
+  <dimension ref="A1:Z991"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -1894,96 +1955,96 @@
         <v>42</v>
       </c>
     </row>
-    <row r="18" spans="1:3" ht="14.25" customHeight="1"/>
+    <row r="18" spans="1:3" ht="14.25" customHeight="1">
+      <c r="A18" t="s">
+        <v>75</v>
+      </c>
+      <c r="B18" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="19" spans="1:3" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>45</v>
+        <v>85</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:3" ht="14.25" customHeight="1">
-      <c r="A20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B20" t="s">
-        <v>47</v>
-      </c>
-      <c r="C20" t="s">
-        <v>49</v>
-      </c>
-    </row>
+    <row r="20" spans="1:3" ht="14.25" customHeight="1"/>
     <row r="21" spans="1:3" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>50</v>
+        <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="14.25" customHeight="1">
       <c r="A22" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B22" t="s">
-        <v>53</v>
+        <v>47</v>
+      </c>
+      <c r="C22" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="14.25" customHeight="1">
       <c r="A23" t="s">
-        <v>54</v>
+        <v>50</v>
       </c>
       <c r="B23" t="s">
-        <v>55</v>
+        <v>48</v>
+      </c>
+      <c r="C23" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="24" spans="1:3" ht="14.25" customHeight="1">
       <c r="A24" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
       <c r="B24" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="14.25" customHeight="1">
       <c r="A25" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
       <c r="B25" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="14.25" customHeight="1">
       <c r="A26" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="14.25" customHeight="1">
       <c r="A27" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B27" t="s">
-        <v>66</v>
+        <v>59</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="14.25" customHeight="1">
       <c r="A28" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B28" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="14.25" customHeight="1">
       <c r="A29" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="B29" t="s">
         <v>65</v>
@@ -1991,38 +2052,52 @@
     </row>
     <row r="30" spans="1:3" ht="14.25" customHeight="1">
       <c r="A30" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B30" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="14.25" customHeight="1">
       <c r="A31" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
       <c r="B31" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="14.25" customHeight="1">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
       <c r="B32" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:2" ht="14.25" customHeight="1">
       <c r="A33" t="s">
+        <v>69</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A34" t="s">
+        <v>71</v>
+      </c>
+      <c r="B34" t="s">
         <v>73</v>
       </c>
-      <c r="B33" t="s">
-        <v>75</v>
-      </c>
     </row>
-    <row r="34" spans="1:2" ht="14.25" customHeight="1"/>
-    <row r="35" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="35" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A35" t="s">
+        <v>72</v>
+      </c>
+      <c r="B35" t="s">
+        <v>74</v>
+      </c>
+    </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="37" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="38" spans="1:2" ht="14.25" customHeight="1"/>
@@ -2977,6 +3052,8 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
     <row r="989" ht="14.25" customHeight="1"/>
+    <row r="990" ht="14.25" customHeight="1"/>
+    <row r="991" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Retry Scope for Line items search
</commit_message>
<xml_diff>
--- a/Extraction_PO_Data_IntoCSV/Data/Config.xlsx
+++ b/Extraction_PO_Data_IntoCSV/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rpa.uat\Documents\UiPath\SH-Cogent\Extraction_PO_Data_IntoCSV\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BCF8B9AD-006C-455E-BDCA-AB880770BA1B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA29BCF8-14C8-4EAB-A8E3-5B941E871464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="117">
   <si>
     <t>Name</t>
   </si>
@@ -342,12 +342,6 @@
     <t>00:00:30</t>
   </si>
   <si>
-    <t>2022.12.14</t>
-  </si>
-  <si>
-    <t>2023.12.14</t>
-  </si>
-  <si>
     <t>SFTP_Host</t>
   </si>
   <si>
@@ -370,6 +364,18 @@
   </si>
   <si>
     <t>SAP__PurchaseorderItems__</t>
+  </si>
+  <si>
+    <t>2022.12.26</t>
+  </si>
+  <si>
+    <t>2023.12.26</t>
+  </si>
+  <si>
+    <t>SFTP_Cred</t>
+  </si>
+  <si>
+    <t>SFTP_Cred_Dev</t>
   </si>
 </sst>
 </file>
@@ -746,10 +752,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z995"/>
+  <dimension ref="A1:Z996"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -870,90 +876,97 @@
     </row>
     <row r="11" spans="1:26" ht="14.25" customHeight="1">
       <c r="A11" t="s">
-        <v>107</v>
+        <v>115</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:26" ht="14.25" customHeight="1">
       <c r="A12" t="s">
-        <v>109</v>
-      </c>
-      <c r="B12">
+        <v>105</v>
+      </c>
+      <c r="B12" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A13" t="s">
+        <v>107</v>
+      </c>
+      <c r="B13">
         <v>22</v>
-      </c>
-    </row>
-    <row r="13" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A13" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B13" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="B14" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" ht="14.25" customHeight="1">
+      <c r="A15" s="2" t="s">
         <v>83</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26" ht="14.25" customHeight="1">
-      <c r="A15" t="s">
-        <v>110</v>
-      </c>
-      <c r="B15" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" t="s">
-        <v>90</v>
+        <v>108</v>
       </c>
       <c r="B16" t="s">
-        <v>96</v>
+        <v>109</v>
       </c>
     </row>
     <row r="17" spans="1:2" ht="14.25" customHeight="1">
       <c r="A17" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
     </row>
     <row r="18" spans="1:2" ht="14.25" customHeight="1">
       <c r="A18" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B18" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="19" spans="1:2" ht="14.25" customHeight="1">
       <c r="A19" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="20" spans="1:2" ht="14.25" customHeight="1">
       <c r="A20" t="s">
-        <v>81</v>
+        <v>93</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>97</v>
       </c>
     </row>
     <row r="21" spans="1:2" ht="14.25" customHeight="1">
       <c r="A21" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="B21" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="14.25" customHeight="1"/>
+    <row r="22" spans="1:2" ht="14.25" customHeight="1">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22" t="s">
+        <v>82</v>
+      </c>
+    </row>
     <row r="23" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="24" spans="1:2" ht="14.25" customHeight="1"/>
     <row r="25" spans="1:2" ht="14.25" customHeight="1"/>
@@ -1927,6 +1940,7 @@
     <row r="993" ht="14.25" customHeight="1"/>
     <row r="994" ht="14.25" customHeight="1"/>
     <row r="995" ht="14.25" customHeight="1"/>
+    <row r="996" ht="14.25" customHeight="1"/>
   </sheetData>
   <phoneticPr fontId="2"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1939,7 +1953,7 @@
   <dimension ref="A1:Z993"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -2169,7 +2183,7 @@
         <v>49</v>
       </c>
       <c r="B24" t="s">
-        <v>105</v>
+        <v>113</v>
       </c>
       <c r="C24" t="s">
         <v>47</v>
@@ -2180,7 +2194,7 @@
         <v>48</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>114</v>
       </c>
       <c r="C25" t="s">
         <v>47</v>
@@ -2255,7 +2269,7 @@
         <v>65</v>
       </c>
       <c r="B34" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="14.25" customHeight="1">
@@ -2263,7 +2277,7 @@
         <v>66</v>
       </c>
       <c r="B35" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="36" spans="1:2" ht="14.25" customHeight="1">
@@ -2287,7 +2301,7 @@
         <v>86</v>
       </c>
       <c r="B38" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="39" spans="1:2" ht="14.25" customHeight="1">

</xml_diff>